<commit_message>
Refactor Code and add new feature
Co-authored-by: Anto Wiranto <antowrnto11@gmail.com>
</commit_message>
<xml_diff>
--- a/storage/aruskas-keuangan-2022.xlsx
+++ b/storage/aruskas-keuangan-2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
   <si>
     <t>I. AKTIVITAS OPERASI</t>
   </si>
@@ -41,10 +41,10 @@
     <t>SD DES 2021</t>
   </si>
   <si>
-    <t>Aug 2022</t>
-  </si>
-  <si>
-    <t>SD Aug 2022</t>
+    <t>Sep 2022</t>
+  </si>
+  <si>
+    <t>SD Sep 2022</t>
   </si>
   <si>
     <t>1. Pengembalian Pinjaman Mitra Binaan</t>
@@ -110,7 +110,7 @@
     <t>2,267,959,574</t>
   </si>
   <si>
-    <t>123,312,144</t>
+    <t>141,680,583</t>
   </si>
   <si>
     <t>13,658,000</t>
@@ -134,22 +134,28 @@
     <t>-2,255,000,000</t>
   </si>
   <si>
+    <t>-317,225</t>
+  </si>
+  <si>
+    <t>-4,176,647</t>
+  </si>
+  <si>
+    <t>-910,000</t>
+  </si>
+  <si>
+    <t>-63,807,932</t>
+  </si>
+  <si>
+    <t>184,524,906</t>
+  </si>
+  <si>
     <t>570,000,000</t>
   </si>
   <si>
-    <t>-317,225</t>
-  </si>
-  <si>
-    <t>-4,176,647</t>
-  </si>
-  <si>
-    <t>-910,000</t>
-  </si>
-  <si>
-    <t>-63,807,932</t>
-  </si>
-  <si>
-    <t>184,524,906</t>
+    <t>11,867,642</t>
+  </si>
+  <si>
+    <t>581,867,642</t>
   </si>
   <si>
     <t>390,508,462</t>
@@ -158,19 +164,19 @@
     <t>142,175,624</t>
   </si>
   <si>
-    <t>658,493,278</t>
-  </si>
-  <si>
-    <t>701,398,798</t>
+    <t>756,829,644</t>
+  </si>
+  <si>
+    <t>1,458,228,442</t>
   </si>
   <si>
     <t>326,700,530</t>
   </si>
   <si>
-    <t>1,228,493,278</t>
-  </si>
-  <si>
-    <t>1,271,398,798</t>
+    <t>768,697,286</t>
+  </si>
+  <si>
+    <t>2,040,096,084</t>
   </si>
 </sst>
 </file>
@@ -684,8 +690,8 @@
       <c r="C12" t="s">
         <v>38</v>
       </c>
-      <c r="D12" t="s">
-        <v>39</v>
+      <c r="D12">
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -764,10 +770,10 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
         <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -801,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -815,16 +821,16 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
         <v>43</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
         <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -876,16 +882,16 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
         <v>43</v>
       </c>
-      <c r="C25" t="s">
-        <v>44</v>
-      </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -893,16 +899,16 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -910,16 +916,16 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>